<commit_message>
Mark mosquito net questions as required
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_mosquito_net/forms/hh_mosquito_net/hh_mosquito_net.xlsx
+++ b/odkx/app/config/tables/hh_mosquito_net/forms/hh_mosquito_net/hh_mosquito_net.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="109">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">display.prompt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required</t>
   </si>
   <si>
     <t xml:space="preserve">select_one</t>
@@ -516,7 +519,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -555,13 +558,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.37"/>
@@ -586,50 +589,62 @@
       <c r="E1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -654,7 +669,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.22"/>
@@ -662,156 +677,156 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -832,11 +847,11 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.5"/>
@@ -850,71 +865,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>20210304001</v>
+        <v>20210421001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>7</v>
@@ -922,49 +937,49 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -992,7 +1007,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.34"/>
@@ -1012,34 +1027,34 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1064,7 +1079,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.56"/>
@@ -1072,226 +1087,226 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>